<commit_message>
some changes and report
</commit_message>
<xml_diff>
--- a/second_version/webscraping/bxl_to_sao/booking_23_may_10_PM.xlsx
+++ b/second_version/webscraping/bxl_to_sao/booking_23_may_10_PM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="94">
   <si>
     <t>out_airline_company</t>
   </si>
@@ -79,7 +79,10 @@
     <t>Lufthansa, operated by Cityjet For Brussels Airlines</t>
   </si>
   <si>
-    <t>KLM</t>
+    <t>Lufthansa, operated by City Jet For Brussels Airlines</t>
+  </si>
+  <si>
+    <t>Lufthansa, operated by Brussels Airlines</t>
   </si>
   <si>
     <t>Swiss</t>
@@ -115,7 +118,16 @@
     <t>1:15 PM</t>
   </si>
   <si>
-    <t>10:25 AM</t>
+    <t>11:20 AM</t>
+  </si>
+  <si>
+    <t>9:30 AM</t>
+  </si>
+  <si>
+    <t>8:15 AM</t>
+  </si>
+  <si>
+    <t>7:00 AM</t>
   </si>
   <si>
     <t>8:15 PM</t>
@@ -148,6 +160,18 @@
     <t>20h 35m</t>
   </si>
   <si>
+    <t>22h 30m</t>
+  </si>
+  <si>
+    <t>24h 20m</t>
+  </si>
+  <si>
+    <t>25h 35m</t>
+  </si>
+  <si>
+    <t>26h 50m</t>
+  </si>
+  <si>
     <t>14h 10m</t>
   </si>
   <si>
@@ -196,6 +220,12 @@
     <t>20h 05m</t>
   </si>
   <si>
+    <t>32h 20m</t>
+  </si>
+  <si>
+    <t>33h 20m</t>
+  </si>
+  <si>
     <t>14h 30m</t>
   </si>
   <si>
@@ -226,6 +256,12 @@
     <t>7:20 PM</t>
   </si>
   <si>
+    <t>7:35 AM</t>
+  </si>
+  <si>
+    <t>8:35 AM</t>
+  </si>
+  <si>
     <t>2:15 PM</t>
   </si>
   <si>
@@ -247,10 +283,16 @@
     <t>2 315,71 €</t>
   </si>
   <si>
+    <t>2 066,05 €</t>
+  </si>
+  <si>
     <t>1 800,01 €</t>
   </si>
   <si>
     <t>1 944,53 €</t>
+  </si>
+  <si>
+    <t>2 094,53 €</t>
   </si>
   <si>
     <t>2 049,51 €</t>
@@ -611,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -684,49 +726,49 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="Q2" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="R2">
         <v>22</v>
@@ -743,49 +785,49 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="N3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="Q3" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="R3">
         <v>22</v>
@@ -802,49 +844,49 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O4" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P4" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="Q4" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R4">
         <v>22</v>
@@ -861,49 +903,49 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O5" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P5" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="Q5" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R5">
         <v>22</v>
@@ -920,49 +962,49 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L6" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M6" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O6" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P6" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="Q6" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="R6">
         <v>22</v>
@@ -979,49 +1021,49 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M7" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="N7" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O7" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P7" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R7">
         <v>22</v>
@@ -1038,49 +1080,49 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K8" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O8" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P8" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="Q8" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="R8">
         <v>22</v>
@@ -1097,49 +1139,49 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="N9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O9" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P9" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q9" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R9">
         <v>22</v>
@@ -1156,49 +1198,49 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="N10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O10" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P10" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q10" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R10">
         <v>22</v>
@@ -1215,49 +1257,49 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L11" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M11" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="N11" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O11" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P11" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="Q11" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="R11">
         <v>22</v>
@@ -1274,49 +1316,49 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M12" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O12" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P12" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="Q12" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R12">
         <v>22</v>
@@ -1333,49 +1375,49 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I13" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L13" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="N13" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O13" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="Q13" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="R13">
         <v>22</v>
@@ -1392,49 +1434,49 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L14" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M14" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="N14" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O14" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P14" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="Q14" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R14">
         <v>22</v>
@@ -1451,49 +1493,49 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L15" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="M15" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="N15" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O15" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P15" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Q15" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="R15">
         <v>22</v>
@@ -1507,52 +1549,52 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
         <v>44</v>
       </c>
       <c r="H16" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L16" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M16" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="N16" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O16" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P16" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="Q16" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R16">
         <v>22</v>
@@ -1563,55 +1605,55 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I17" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L17" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M17" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="N17" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O17" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P17" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="Q17" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R17">
         <v>22</v>
@@ -1622,55 +1664,55 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M18" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="N18" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O18" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="P18" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="Q18" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="R18">
         <v>22</v>
@@ -1681,55 +1723,55 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I19" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J19" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K19" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L19" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M19" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="N19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O19" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P19" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="Q19" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R19">
         <v>22</v>
@@ -1740,55 +1782,55 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F20" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J20" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L20" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M20" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="N20" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O20" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P20" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="Q20" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R20">
         <v>22</v>
@@ -1799,55 +1841,55 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
         <v>45</v>
       </c>
       <c r="H21" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I21" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J21" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K21" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L21" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M21" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="N21" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O21" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P21" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="Q21" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="R21">
         <v>22</v>
@@ -1858,55 +1900,55 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H22" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I22" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J22" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K22" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L22" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M22" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="N22" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="O22" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P22" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="Q22" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R22">
         <v>22</v>
@@ -1917,55 +1959,55 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
         <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I23" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J23" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K23" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L23" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M23" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="N23" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O23" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P23" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="Q23" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R23">
         <v>22</v>
@@ -1976,55 +2018,55 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I24" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J24" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K24" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L24" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M24" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="N24" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O24" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P24" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="Q24" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="R24">
         <v>22</v>
@@ -2035,55 +2077,55 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G25" t="s">
         <v>47</v>
       </c>
       <c r="H25" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I25" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J25" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K25" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L25" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M25" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="N25" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O25" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P25" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="Q25" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="R25">
         <v>22</v>
@@ -2094,55 +2136,55 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I26" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J26" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K26" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L26" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M26" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="N26" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O26" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="P26" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="Q26" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R26">
         <v>22</v>
@@ -2153,55 +2195,55 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F27" t="s">
         <v>34</v>
       </c>
       <c r="G27" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H27" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I27" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J27" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K27" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L27" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M27" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="N27" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O27" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="P27" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="Q27" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="R27">
         <v>22</v>
@@ -2212,55 +2254,55 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H28" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="I28" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J28" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K28" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L28" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="M28" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="N28" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="O28" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="P28" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="Q28" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="R28">
         <v>22</v>
@@ -2271,60 +2313,1712 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" t="s">
+        <v>59</v>
+      </c>
+      <c r="J29" t="s">
+        <v>60</v>
+      </c>
+      <c r="K29" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29" t="s">
+        <v>69</v>
+      </c>
+      <c r="N29" t="s">
+        <v>57</v>
+      </c>
+      <c r="O29" t="s">
+        <v>76</v>
+      </c>
+      <c r="P29" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>89</v>
+      </c>
+      <c r="R29">
+        <v>22</v>
+      </c>
+      <c r="S29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" t="s">
+        <v>59</v>
+      </c>
+      <c r="J30" t="s">
+        <v>60</v>
+      </c>
+      <c r="K30" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" t="s">
+        <v>69</v>
+      </c>
+      <c r="N30" t="s">
+        <v>57</v>
+      </c>
+      <c r="O30" t="s">
+        <v>76</v>
+      </c>
+      <c r="P30" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>89</v>
+      </c>
+      <c r="R30">
+        <v>22</v>
+      </c>
+      <c r="S30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" t="s">
+        <v>59</v>
+      </c>
+      <c r="J31" t="s">
+        <v>60</v>
+      </c>
+      <c r="K31" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" t="s">
+        <v>63</v>
+      </c>
+      <c r="M31" t="s">
+        <v>68</v>
+      </c>
+      <c r="N31" t="s">
+        <v>57</v>
+      </c>
+      <c r="O31" t="s">
+        <v>76</v>
+      </c>
+      <c r="P31" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>89</v>
+      </c>
+      <c r="R31">
+        <v>22</v>
+      </c>
+      <c r="S31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L32" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" t="s">
+        <v>69</v>
+      </c>
+      <c r="N32" t="s">
+        <v>57</v>
+      </c>
+      <c r="O32" t="s">
+        <v>76</v>
+      </c>
+      <c r="P32" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>89</v>
+      </c>
+      <c r="R32">
+        <v>22</v>
+      </c>
+      <c r="S32">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" t="s">
+        <v>62</v>
+      </c>
+      <c r="L33" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" t="s">
+        <v>68</v>
+      </c>
+      <c r="N33" t="s">
+        <v>57</v>
+      </c>
+      <c r="O33" t="s">
+        <v>76</v>
+      </c>
+      <c r="P33" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>89</v>
+      </c>
+      <c r="R33">
+        <v>22</v>
+      </c>
+      <c r="S33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" t="s">
+        <v>61</v>
+      </c>
+      <c r="K34" t="s">
+        <v>62</v>
+      </c>
+      <c r="L34" t="s">
+        <v>64</v>
+      </c>
+      <c r="M34" t="s">
+        <v>70</v>
+      </c>
+      <c r="N34" t="s">
+        <v>57</v>
+      </c>
+      <c r="O34" t="s">
+        <v>75</v>
+      </c>
+      <c r="P34" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>90</v>
+      </c>
+      <c r="R34">
+        <v>22</v>
+      </c>
+      <c r="S34">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J35" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" t="s">
+        <v>62</v>
+      </c>
+      <c r="L35" t="s">
+        <v>64</v>
+      </c>
+      <c r="M35" t="s">
+        <v>71</v>
+      </c>
+      <c r="N35" t="s">
+        <v>57</v>
+      </c>
+      <c r="O35" t="s">
+        <v>75</v>
+      </c>
+      <c r="P35" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>90</v>
+      </c>
+      <c r="R35">
+        <v>22</v>
+      </c>
+      <c r="S35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J36" t="s">
+        <v>61</v>
+      </c>
+      <c r="K36" t="s">
+        <v>62</v>
+      </c>
+      <c r="L36" t="s">
+        <v>64</v>
+      </c>
+      <c r="M36" t="s">
+        <v>70</v>
+      </c>
+      <c r="N36" t="s">
+        <v>57</v>
+      </c>
+      <c r="O36" t="s">
+        <v>75</v>
+      </c>
+      <c r="P36" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>90</v>
+      </c>
+      <c r="R36">
+        <v>22</v>
+      </c>
+      <c r="S36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" t="s">
+        <v>53</v>
+      </c>
+      <c r="H37" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" t="s">
+        <v>59</v>
+      </c>
+      <c r="J37" t="s">
+        <v>61</v>
+      </c>
+      <c r="K37" t="s">
+        <v>62</v>
+      </c>
+      <c r="L37" t="s">
+        <v>64</v>
+      </c>
+      <c r="M37" t="s">
+        <v>71</v>
+      </c>
+      <c r="N37" t="s">
+        <v>57</v>
+      </c>
+      <c r="O37" t="s">
+        <v>75</v>
+      </c>
+      <c r="P37" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>90</v>
+      </c>
+      <c r="R37">
+        <v>22</v>
+      </c>
+      <c r="S37">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" t="s">
+        <v>59</v>
+      </c>
+      <c r="J38" t="s">
+        <v>61</v>
+      </c>
+      <c r="K38" t="s">
+        <v>62</v>
+      </c>
+      <c r="L38" t="s">
+        <v>64</v>
+      </c>
+      <c r="M38" t="s">
+        <v>70</v>
+      </c>
+      <c r="N38" t="s">
+        <v>57</v>
+      </c>
+      <c r="O38" t="s">
+        <v>75</v>
+      </c>
+      <c r="P38" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>90</v>
+      </c>
+      <c r="R38">
+        <v>22</v>
+      </c>
+      <c r="S38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" t="s">
         <v>25</v>
       </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" t="s">
+        <v>58</v>
+      </c>
+      <c r="I39" t="s">
+        <v>59</v>
+      </c>
+      <c r="J39" t="s">
+        <v>61</v>
+      </c>
+      <c r="K39" t="s">
+        <v>62</v>
+      </c>
+      <c r="L39" t="s">
+        <v>64</v>
+      </c>
+      <c r="M39" t="s">
+        <v>70</v>
+      </c>
+      <c r="N39" t="s">
+        <v>57</v>
+      </c>
+      <c r="O39" t="s">
+        <v>75</v>
+      </c>
+      <c r="P39" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>91</v>
+      </c>
+      <c r="R39">
+        <v>22</v>
+      </c>
+      <c r="S39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
         <v>38</v>
       </c>
-      <c r="G29" t="s">
-        <v>48</v>
-      </c>
-      <c r="H29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I29" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" t="s">
+        <v>59</v>
+      </c>
+      <c r="J40" t="s">
+        <v>61</v>
+      </c>
+      <c r="K40" t="s">
+        <v>62</v>
+      </c>
+      <c r="L40" t="s">
+        <v>64</v>
+      </c>
+      <c r="M40" t="s">
+        <v>72</v>
+      </c>
+      <c r="N40" t="s">
+        <v>58</v>
+      </c>
+      <c r="O40" t="s">
+        <v>75</v>
+      </c>
+      <c r="P40" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>92</v>
+      </c>
+      <c r="R40">
+        <v>22</v>
+      </c>
+      <c r="S40">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s">
+        <v>40</v>
+      </c>
+      <c r="G41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H41" t="s">
+        <v>57</v>
+      </c>
+      <c r="I41" t="s">
+        <v>59</v>
+      </c>
+      <c r="J41" t="s">
+        <v>61</v>
+      </c>
+      <c r="K41" t="s">
+        <v>62</v>
+      </c>
+      <c r="L41" t="s">
+        <v>64</v>
+      </c>
+      <c r="M41" t="s">
+        <v>71</v>
+      </c>
+      <c r="N41" t="s">
+        <v>57</v>
+      </c>
+      <c r="O41" t="s">
+        <v>75</v>
+      </c>
+      <c r="P41" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>90</v>
+      </c>
+      <c r="R41">
+        <v>22</v>
+      </c>
+      <c r="S41">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" t="s">
         <v>53</v>
       </c>
-      <c r="K29" t="s">
+      <c r="H42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I42" t="s">
+        <v>59</v>
+      </c>
+      <c r="J42" t="s">
+        <v>61</v>
+      </c>
+      <c r="K42" t="s">
+        <v>62</v>
+      </c>
+      <c r="L42" t="s">
+        <v>64</v>
+      </c>
+      <c r="M42" t="s">
+        <v>71</v>
+      </c>
+      <c r="N42" t="s">
+        <v>57</v>
+      </c>
+      <c r="O42" t="s">
+        <v>75</v>
+      </c>
+      <c r="P42" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>92</v>
+      </c>
+      <c r="R42">
+        <v>22</v>
+      </c>
+      <c r="S42">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s">
+        <v>41</v>
+      </c>
+      <c r="G43" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" t="s">
+        <v>58</v>
+      </c>
+      <c r="I43" t="s">
+        <v>59</v>
+      </c>
+      <c r="J43" t="s">
+        <v>61</v>
+      </c>
+      <c r="K43" t="s">
+        <v>62</v>
+      </c>
+      <c r="L43" t="s">
+        <v>64</v>
+      </c>
+      <c r="M43" t="s">
+        <v>70</v>
+      </c>
+      <c r="N43" t="s">
+        <v>57</v>
+      </c>
+      <c r="O43" t="s">
+        <v>75</v>
+      </c>
+      <c r="P43" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>91</v>
+      </c>
+      <c r="R43">
+        <v>22</v>
+      </c>
+      <c r="S43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G44" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" t="s">
+        <v>58</v>
+      </c>
+      <c r="I44" t="s">
+        <v>59</v>
+      </c>
+      <c r="J44" t="s">
+        <v>61</v>
+      </c>
+      <c r="K44" t="s">
+        <v>62</v>
+      </c>
+      <c r="L44" t="s">
+        <v>64</v>
+      </c>
+      <c r="M44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N44" t="s">
+        <v>57</v>
+      </c>
+      <c r="O44" t="s">
+        <v>75</v>
+      </c>
+      <c r="P44" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>91</v>
+      </c>
+      <c r="R44">
+        <v>22</v>
+      </c>
+      <c r="S44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" t="s">
+        <v>52</v>
+      </c>
+      <c r="H45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I45" t="s">
+        <v>59</v>
+      </c>
+      <c r="J45" t="s">
+        <v>61</v>
+      </c>
+      <c r="K45" t="s">
+        <v>62</v>
+      </c>
+      <c r="L45" t="s">
+        <v>64</v>
+      </c>
+      <c r="M45" t="s">
+        <v>73</v>
+      </c>
+      <c r="N45" t="s">
+        <v>57</v>
+      </c>
+      <c r="O45" t="s">
+        <v>76</v>
+      </c>
+      <c r="P45" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>91</v>
+      </c>
+      <c r="R45">
+        <v>22</v>
+      </c>
+      <c r="S45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H46" t="s">
+        <v>57</v>
+      </c>
+      <c r="I46" t="s">
+        <v>59</v>
+      </c>
+      <c r="J46" t="s">
+        <v>61</v>
+      </c>
+      <c r="K46" t="s">
+        <v>62</v>
+      </c>
+      <c r="L46" t="s">
+        <v>64</v>
+      </c>
+      <c r="M46" t="s">
+        <v>74</v>
+      </c>
+      <c r="N46" t="s">
+        <v>57</v>
+      </c>
+      <c r="O46" t="s">
+        <v>76</v>
+      </c>
+      <c r="P46" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>90</v>
+      </c>
+      <c r="R46">
+        <v>22</v>
+      </c>
+      <c r="S46">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" t="s">
+        <v>56</v>
+      </c>
+      <c r="H47" t="s">
+        <v>57</v>
+      </c>
+      <c r="I47" t="s">
+        <v>59</v>
+      </c>
+      <c r="J47" t="s">
+        <v>61</v>
+      </c>
+      <c r="K47" t="s">
+        <v>62</v>
+      </c>
+      <c r="L47" t="s">
+        <v>64</v>
+      </c>
+      <c r="M47" t="s">
+        <v>70</v>
+      </c>
+      <c r="N47" t="s">
+        <v>57</v>
+      </c>
+      <c r="O47" t="s">
+        <v>75</v>
+      </c>
+      <c r="P47" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>93</v>
+      </c>
+      <c r="R47">
+        <v>22</v>
+      </c>
+      <c r="S47">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48" t="s">
+        <v>57</v>
+      </c>
+      <c r="I48" t="s">
+        <v>59</v>
+      </c>
+      <c r="J48" t="s">
+        <v>61</v>
+      </c>
+      <c r="K48" t="s">
+        <v>62</v>
+      </c>
+      <c r="L48" t="s">
+        <v>64</v>
+      </c>
+      <c r="M48" t="s">
+        <v>74</v>
+      </c>
+      <c r="N48" t="s">
+        <v>57</v>
+      </c>
+      <c r="O48" t="s">
+        <v>76</v>
+      </c>
+      <c r="P48" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>90</v>
+      </c>
+      <c r="R48">
+        <v>22</v>
+      </c>
+      <c r="S48">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" t="s">
+        <v>56</v>
+      </c>
+      <c r="H49" t="s">
+        <v>57</v>
+      </c>
+      <c r="I49" t="s">
+        <v>59</v>
+      </c>
+      <c r="J49" t="s">
+        <v>61</v>
+      </c>
+      <c r="K49" t="s">
+        <v>62</v>
+      </c>
+      <c r="L49" t="s">
+        <v>64</v>
+      </c>
+      <c r="M49" t="s">
+        <v>71</v>
+      </c>
+      <c r="N49" t="s">
+        <v>57</v>
+      </c>
+      <c r="O49" t="s">
+        <v>75</v>
+      </c>
+      <c r="P49" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>93</v>
+      </c>
+      <c r="R49">
+        <v>22</v>
+      </c>
+      <c r="S49">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" t="s">
         <v>54</v>
       </c>
-      <c r="L29" t="s">
+      <c r="H50" t="s">
+        <v>57</v>
+      </c>
+      <c r="I50" t="s">
+        <v>59</v>
+      </c>
+      <c r="J50" t="s">
+        <v>61</v>
+      </c>
+      <c r="K50" t="s">
+        <v>62</v>
+      </c>
+      <c r="L50" t="s">
+        <v>64</v>
+      </c>
+      <c r="M50" t="s">
+        <v>73</v>
+      </c>
+      <c r="N50" t="s">
+        <v>57</v>
+      </c>
+      <c r="O50" t="s">
+        <v>76</v>
+      </c>
+      <c r="P50" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>90</v>
+      </c>
+      <c r="R50">
+        <v>22</v>
+      </c>
+      <c r="S50">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G51" t="s">
+        <v>54</v>
+      </c>
+      <c r="H51" t="s">
+        <v>57</v>
+      </c>
+      <c r="I51" t="s">
+        <v>59</v>
+      </c>
+      <c r="J51" t="s">
+        <v>61</v>
+      </c>
+      <c r="K51" t="s">
+        <v>62</v>
+      </c>
+      <c r="L51" t="s">
+        <v>64</v>
+      </c>
+      <c r="M51" t="s">
+        <v>74</v>
+      </c>
+      <c r="N51" t="s">
+        <v>57</v>
+      </c>
+      <c r="O51" t="s">
+        <v>76</v>
+      </c>
+      <c r="P51" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>90</v>
+      </c>
+      <c r="R51">
+        <v>22</v>
+      </c>
+      <c r="S51">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" t="s">
+        <v>42</v>
+      </c>
+      <c r="G52" t="s">
         <v>56</v>
       </c>
-      <c r="M29" t="s">
-        <v>60</v>
-      </c>
-      <c r="N29" t="s">
-        <v>49</v>
-      </c>
-      <c r="O29" t="s">
-        <v>65</v>
-      </c>
-      <c r="P29" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R29">
-        <v>22</v>
-      </c>
-      <c r="S29">
+      <c r="H52" t="s">
+        <v>57</v>
+      </c>
+      <c r="I52" t="s">
+        <v>59</v>
+      </c>
+      <c r="J52" t="s">
+        <v>61</v>
+      </c>
+      <c r="K52" t="s">
+        <v>62</v>
+      </c>
+      <c r="L52" t="s">
+        <v>64</v>
+      </c>
+      <c r="M52" t="s">
+        <v>73</v>
+      </c>
+      <c r="N52" t="s">
+        <v>57</v>
+      </c>
+      <c r="O52" t="s">
+        <v>76</v>
+      </c>
+      <c r="P52" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>93</v>
+      </c>
+      <c r="R52">
+        <v>22</v>
+      </c>
+      <c r="S52">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53" t="s">
+        <v>39</v>
+      </c>
+      <c r="G53" t="s">
+        <v>53</v>
+      </c>
+      <c r="H53" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" t="s">
+        <v>59</v>
+      </c>
+      <c r="J53" t="s">
+        <v>61</v>
+      </c>
+      <c r="K53" t="s">
+        <v>62</v>
+      </c>
+      <c r="L53" t="s">
+        <v>64</v>
+      </c>
+      <c r="M53" t="s">
+        <v>74</v>
+      </c>
+      <c r="N53" t="s">
+        <v>57</v>
+      </c>
+      <c r="O53" t="s">
+        <v>76</v>
+      </c>
+      <c r="P53" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>90</v>
+      </c>
+      <c r="R53">
+        <v>22</v>
+      </c>
+      <c r="S53">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H54" t="s">
+        <v>57</v>
+      </c>
+      <c r="I54" t="s">
+        <v>59</v>
+      </c>
+      <c r="J54" t="s">
+        <v>61</v>
+      </c>
+      <c r="K54" t="s">
+        <v>62</v>
+      </c>
+      <c r="L54" t="s">
+        <v>64</v>
+      </c>
+      <c r="M54" t="s">
+        <v>71</v>
+      </c>
+      <c r="N54" t="s">
+        <v>57</v>
+      </c>
+      <c r="O54" t="s">
+        <v>75</v>
+      </c>
+      <c r="P54" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>93</v>
+      </c>
+      <c r="R54">
+        <v>22</v>
+      </c>
+      <c r="S54">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" t="s">
+        <v>54</v>
+      </c>
+      <c r="H55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I55" t="s">
+        <v>59</v>
+      </c>
+      <c r="J55" t="s">
+        <v>61</v>
+      </c>
+      <c r="K55" t="s">
+        <v>62</v>
+      </c>
+      <c r="L55" t="s">
+        <v>64</v>
+      </c>
+      <c r="M55" t="s">
+        <v>73</v>
+      </c>
+      <c r="N55" t="s">
+        <v>57</v>
+      </c>
+      <c r="O55" t="s">
+        <v>76</v>
+      </c>
+      <c r="P55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>90</v>
+      </c>
+      <c r="R55">
+        <v>22</v>
+      </c>
+      <c r="S55">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="A56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" t="s">
+        <v>40</v>
+      </c>
+      <c r="G56" t="s">
+        <v>54</v>
+      </c>
+      <c r="H56" t="s">
+        <v>57</v>
+      </c>
+      <c r="I56" t="s">
+        <v>59</v>
+      </c>
+      <c r="J56" t="s">
+        <v>61</v>
+      </c>
+      <c r="K56" t="s">
+        <v>62</v>
+      </c>
+      <c r="L56" t="s">
+        <v>64</v>
+      </c>
+      <c r="M56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N56" t="s">
+        <v>57</v>
+      </c>
+      <c r="O56" t="s">
+        <v>76</v>
+      </c>
+      <c r="P56" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>90</v>
+      </c>
+      <c r="R56">
+        <v>22</v>
+      </c>
+      <c r="S56">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" t="s">
+        <v>42</v>
+      </c>
+      <c r="G57" t="s">
+        <v>56</v>
+      </c>
+      <c r="H57" t="s">
+        <v>57</v>
+      </c>
+      <c r="I57" t="s">
+        <v>59</v>
+      </c>
+      <c r="J57" t="s">
+        <v>61</v>
+      </c>
+      <c r="K57" t="s">
+        <v>62</v>
+      </c>
+      <c r="L57" t="s">
+        <v>64</v>
+      </c>
+      <c r="M57" t="s">
+        <v>73</v>
+      </c>
+      <c r="N57" t="s">
+        <v>57</v>
+      </c>
+      <c r="O57" t="s">
+        <v>76</v>
+      </c>
+      <c r="P57" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>93</v>
+      </c>
+      <c r="R57">
+        <v>22</v>
+      </c>
+      <c r="S57">
         <v>23</v>
       </c>
     </row>

</xml_diff>